<commit_message>
EntityType with Integration Workflow
</commit_message>
<xml_diff>
--- a/Lexis-GLOBAL/Coredata/ENTITY_TYPE.xlsx
+++ b/Lexis-GLOBAL/Coredata/ENTITY_TYPE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adapp\git\AutoAPI\Lexis-GLOBAL\Coredata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919C19E9-4DF9-4DAF-BB0A-5A8479321A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5B3C43-DB3D-499F-A3CD-A0109F79D22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="599" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EntityType_View" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="38">
   <si>
     <t>S.No</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>CREATE</t>
   </si>
 </sst>
 </file>
@@ -515,7 +524,170 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="18.08984375" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" customWidth="1"/>
+    <col min="8" max="9" width="18.08984375" customWidth="1"/>
+    <col min="10" max="10" width="20.7265625" customWidth="1"/>
+    <col min="11" max="11" width="18.26953125" customWidth="1"/>
+    <col min="12" max="12" width="27.1796875" hidden="1" customWidth="1"/>
+    <col min="13" max="16" width="18.08984375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="21.81640625" customWidth="1"/>
+    <col min="18" max="18" width="19.6328125" customWidth="1"/>
+    <col min="19" max="19" width="9.81640625" customWidth="1"/>
+    <col min="20" max="20" width="15.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="K9" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58177AC0-248F-40FE-9FDD-59CC7E7A6771}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -669,16 +841,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58177AC0-248F-40FE-9FDD-59CC7E7A6771}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7022E7C1-82BB-480E-BECC-5D14C5961F65}">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -770,7 +941,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>21</v>
@@ -835,12 +1006,175 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7022E7C1-82BB-480E-BECC-5D14C5961F65}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162A4AFC-9F81-4D4B-B7E3-21F3F5FF0F13}">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" customWidth="1"/>
+    <col min="8" max="9" width="18.08984375" customWidth="1"/>
+    <col min="10" max="10" width="20.7265625" customWidth="1"/>
+    <col min="11" max="11" width="18.26953125" customWidth="1"/>
+    <col min="12" max="12" width="27.1796875" hidden="1" customWidth="1"/>
+    <col min="13" max="16" width="18.08984375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="21.81640625" customWidth="1"/>
+    <col min="18" max="18" width="19.6328125" customWidth="1"/>
+    <col min="19" max="19" width="9.81640625" customWidth="1"/>
+    <col min="20" max="20" width="15.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="K9" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBD611E-B291-4486-A739-CD803A429250}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -932,331 +1266,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="4"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="K9" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162A4AFC-9F81-4D4B-B7E3-21F3F5FF0F13}">
-  <dimension ref="A1:T9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="18.08984375" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="19.26953125" customWidth="1"/>
-    <col min="7" max="7" width="17.08984375" customWidth="1"/>
-    <col min="8" max="9" width="18.08984375" customWidth="1"/>
-    <col min="10" max="10" width="20.7265625" customWidth="1"/>
-    <col min="11" max="11" width="18.26953125" customWidth="1"/>
-    <col min="12" max="12" width="27.1796875" customWidth="1"/>
-    <col min="13" max="16" width="18.08984375" customWidth="1"/>
-    <col min="17" max="17" width="21.81640625" customWidth="1"/>
-    <col min="18" max="18" width="19.6328125" customWidth="1"/>
-    <col min="19" max="19" width="9.81640625" customWidth="1"/>
-    <col min="20" max="20" width="15.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="4"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="K9" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBD611E-B291-4486-A739-CD803A429250}">
-  <dimension ref="A1:T9"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="18.08984375" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="19.26953125" customWidth="1"/>
-    <col min="7" max="7" width="17.08984375" customWidth="1"/>
-    <col min="8" max="9" width="18.08984375" customWidth="1"/>
-    <col min="10" max="10" width="20.7265625" customWidth="1"/>
-    <col min="11" max="11" width="18.26953125" customWidth="1"/>
-    <col min="12" max="12" width="27.1796875" customWidth="1"/>
-    <col min="13" max="16" width="18.08984375" customWidth="1"/>
-    <col min="17" max="17" width="21.81640625" customWidth="1"/>
-    <col min="18" max="18" width="19.6328125" customWidth="1"/>
-    <col min="19" max="19" width="9.81640625" customWidth="1"/>
-    <col min="20" max="20" width="15.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>21</v>

</xml_diff>